<commit_message>
演習２および3が完成！# This is a combination of 6 commits.
[演習２が完成！]コードレビューも完了

[演習３]Viewを作成

[演習3]ドメインクラスを作成wq

[演習３]リポジトリクラスの性別＆色検索を実装

[演習3]動作確認完了、テストに入る

[演習3]テスト完了
</commit_message>
<xml_diff>
--- a/Document/演習２テスト仕様書.xlsx
+++ b/Document/演習２テスト仕様書.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>作成者</t>
     <rPh sb="0" eb="3">
@@ -132,19 +132,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Spring中級：演習１　ブラックボックステスト仕様書</t>
-    <rPh sb="6" eb="8">
-      <t>チュウキュウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>エンシュウ</t>
-    </rPh>
-    <rPh sb="24" eb="27">
-      <t>シヨウショ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">    id serial primary key,</t>
   </si>
   <si>
@@ -241,20 +228,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>リンクに「http://localhost:8080/ex-intermediate/hotelSerch」と入力し検索する</t>
-    <rPh sb="55" eb="57">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ケンサク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ホテル検索画面が表示されていること</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>①入力欄に10000と入力
 ②検索ボタンを押下</t>
     <rPh sb="1" eb="3">
@@ -275,40 +248,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>以下の順番で3件のホテルが表示されていること
--横浜ベイホテル東京
--渋谷エクセルホテル東京
--ホテルローズガーデン東京</t>
-    <rPh sb="0" eb="2">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ジュンバン</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ケン</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ヨコハマ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>トウキョウ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>シブヤ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>トウキョウ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>トウキョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>空欄で検索した際に全件出力されるか</t>
     <rPh sb="0" eb="1">
       <t>カラ</t>
@@ -348,25 +287,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>全ホテルが価格の高い順で表示されていること</t>
-    <rPh sb="0" eb="1">
-      <t>ゼン</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カカク</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>タカ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ジュン</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>入力系
 （異常系）</t>
     <rPh sb="0" eb="3">
@@ -388,61 +308,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>①入力欄に-1000と入力
-②検索ボタンを押下</t>
-    <rPh sb="1" eb="3">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ラン</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>オウカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「金額を入力してください」とエラー文が表示されていること</t>
-    <rPh sb="1" eb="3">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ブン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ホテルを検索する</t>
     <rPh sb="4" eb="6">
       <t>ケンサク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「数字で入力してください」とエラー文が表示されていること</t>
-    <rPh sb="1" eb="3">
-      <t>スウジ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ブン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -490,20 +358,6 @@
       <t>テキセツ</t>
     </rPh>
     <rPh sb="18" eb="20">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ホテル検索画面が表示されていること
-・1件もデータが存在しませんと表示されていること</t>
-    <rPh sb="20" eb="21">
-      <t>ケン</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ソンザイ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
       <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -535,12 +389,323 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>検索結果が1件もない場合に適切な表示がされるか</t>
+    <rPh sb="0" eb="4">
+      <t>ケンサクケッカ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>テキセツ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①入力欄に「500」と入力
+②検索ボタンを押下</t>
+    <rPh sb="1" eb="4">
+      <t>ニュウリョクラン</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・以下の順番で3件のホテルが表示されていること
+-横浜ベイホテル東京
+-渋谷エクセルホテル東京
+-ホテルローズガーデン東京</t>
+    <rPh sb="20" eb="22">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジュンバン</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヨコハマ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>トウキョウ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>シブヤ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>トウキョウ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>トウキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・「DBに1件もデータが存在しません」と表示されていること</t>
+    <rPh sb="25" eb="26">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ソンザイ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大熊隆寛</t>
+    <rPh sb="0" eb="2">
+      <t>オオクマ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>タカシ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ヒロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・5つのホテルが価格の高い順で表示されていること</t>
+    <rPh sb="27" eb="29">
+      <t>カカク</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ジュン</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・ホテルが何も表示されていないこと</t>
+    <rPh sb="4" eb="8">
+      <t>ケンサクガメン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①入力欄に5000と入力
+②検索ボタンを押下</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・１件のホテルが表示されていること
+-ホテルローズガーデン東京</t>
+    <rPh sb="21" eb="22">
+      <t>ケン</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>トウキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・「金額を半角数字で入力してください」とエラー文が表示されていること</t>
+    <rPh sb="21" eb="23">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="24" eb="28">
+      <t>ハンカクスウジ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>ブン</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Spring中級：演習2　ブラックボックステスト仕様書</t>
+    <rPh sb="6" eb="8">
+      <t>チュウキュウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>エンシュウ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>シヨウショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リンクに「http://localhost:8080/ex-intermediate/hote」と入力しアクセスする</t>
+    <rPh sb="49" eb="51">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リンクに「http://localhost:8081/ex-intermediate/hotel」と入力しアクセスする</t>
+    <rPh sb="50" eb="52">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①入力欄に4999と入力
+②検索ボタンを押下</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・ホテルが何も表示されないこと</t>
+    <rPh sb="24" eb="25">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①入力欄に-1と入力
+②検索ボタンを押下</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①入力欄に0と入力
+②検索ボタンを押下</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>オウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ホテル検索画面が表示されていること
+・ホテルが何も表示されないこと
+※エラー文が出ていないこと</t>
+    <rPh sb="24" eb="25">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ブン</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>デ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,14 +773,6 @@
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -692,7 +849,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -729,11 +886,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -746,9 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,11 +1184,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.375" defaultRowHeight="13.5"/>
@@ -1053,7 +1207,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1115,196 +1269,348 @@
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" ht="58.5" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="11"/>
+      <c r="G4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="12">
+        <v>44343</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="G5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="12">
+        <v>44344</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="81.75" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="12">
+        <v>44343</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="81.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="12">
+        <v>44344</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="9" customFormat="1" ht="81.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="12">
+        <v>44345</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="12">
+        <v>44343</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="12">
+        <v>44344</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="E11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="12">
+        <v>44344</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="12">
+        <v>44345</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="9" customFormat="1" ht="66.75" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" ht="66.75" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="11"/>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="12">
+        <v>44346</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="18"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="2"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" s="9" customFormat="1" ht="60.75" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1320,109 +1626,109 @@
   <dimension ref="A1:A110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1">
@@ -1707,59 +2013,59 @@
   <dimension ref="A1:A110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection sqref="A1:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1">

</xml_diff>